<commit_message>
Import from csv done but not from excel to csv
</commit_message>
<xml_diff>
--- a/SaveEarth/Assets/StaticData/DataID.xlsx
+++ b/SaveEarth/Assets/StaticData/DataID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SaveEarth\SaveEarthFromGlobalWarming\SaveEarth\Assets\StaticData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39B348F-1AE1-4DB3-92C9-D3E487B6744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE62268-0AAA-4F0D-96CF-8AC893EEC280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="3390" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3780" yWindow="2085" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -384,7 +384,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>